<commit_message>
working on pi markers that can be better distinguished -> cross-ratio analysis
</commit_message>
<xml_diff>
--- a/cob_fiducials/common/files/fiducials/pi/Fiducials.xlsx
+++ b/cob_fiducials/common/files/fiducials/pi/Fiducials.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Line 0 (y-axis)</t>
   </si>
@@ -50,6 +49,21 @@
   </si>
   <si>
     <t>useable</t>
+  </si>
+  <si>
+    <t>possible cross ratios:</t>
+  </si>
+  <si>
+    <t>combos:</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>cross ratio similarity with</t>
+  </si>
+  <si>
+    <t>good distance to others</t>
   </si>
 </sst>
 </file>
@@ -91,7 +105,37 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="40">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -109,6 +153,296 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -469,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:W37"/>
+  <dimension ref="B2:W128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,6 +815,8 @@
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:23" x14ac:dyDescent="0.25">
@@ -546,7 +882,7 @@
         <v>80</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I37" si="0">E4*(D4-F4)/((D4-E4)*F4)</f>
+        <f t="shared" ref="I4:I67" si="0">E4*(D4-F4)/((D4-E4)*F4)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="J4">
@@ -820,7 +1156,7 @@
         <v>65</v>
       </c>
       <c r="T9">
-        <f t="shared" si="6"/>
+        <f>P9*(O9-Q9)/((O9-P9)*Q9)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="U9">
@@ -2561,7 +2897,7 @@
         <v>3.8461538461538547E-2</v>
       </c>
     </row>
-    <row r="33" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>29</v>
       </c>
@@ -2636,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>30</v>
       </c>
@@ -2711,7 +3047,7 @@
         <v>0.51948051948051943</v>
       </c>
     </row>
-    <row r="35" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>31</v>
       </c>
@@ -2786,7 +3122,7 @@
         <v>1.4545454545454546</v>
       </c>
     </row>
-    <row r="36" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>32</v>
       </c>
@@ -2861,7 +3197,7 @@
         <v>2.3191094619666064E-2</v>
       </c>
     </row>
-    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>33</v>
       </c>
@@ -2936,25 +3272,2374 @@
         <v>0.57792207792207795</v>
       </c>
     </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I38" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="I39" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>100</v>
+      </c>
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>40</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="F41">
+        <v>45</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>0.30555555555555558</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>100</v>
+      </c>
+      <c r="E42">
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <v>50</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>100</v>
+      </c>
+      <c r="E43">
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <v>55</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>0.20454545454545456</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>100</v>
+      </c>
+      <c r="E44">
+        <v>20</v>
+      </c>
+      <c r="F44">
+        <v>60</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>100</v>
+      </c>
+      <c r="E45">
+        <v>20</v>
+      </c>
+      <c r="F45">
+        <v>65</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>0.13461538461538461</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>100</v>
+      </c>
+      <c r="E46">
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <v>70</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="0"/>
+        <v>0.10714285714285714</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>100</v>
+      </c>
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <v>75</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>100</v>
+      </c>
+      <c r="E48">
+        <v>20</v>
+      </c>
+      <c r="F48">
+        <v>80</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="E49">
+        <v>25</v>
+      </c>
+      <c r="F49">
+        <v>45</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>0.40740740740740738</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>100</v>
+      </c>
+      <c r="E50">
+        <v>25</v>
+      </c>
+      <c r="F50">
+        <v>50</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>100</v>
+      </c>
+      <c r="E51">
+        <v>25</v>
+      </c>
+      <c r="F51">
+        <v>55</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>100</v>
+      </c>
+      <c r="E52">
+        <v>25</v>
+      </c>
+      <c r="F52">
+        <v>60</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>100</v>
+      </c>
+      <c r="E53">
+        <v>25</v>
+      </c>
+      <c r="F53">
+        <v>65</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>0.17948717948717949</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>100</v>
+      </c>
+      <c r="E54">
+        <v>25</v>
+      </c>
+      <c r="F54">
+        <v>70</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>100</v>
+      </c>
+      <c r="E55">
+        <v>25</v>
+      </c>
+      <c r="F55">
+        <v>75</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>100</v>
+      </c>
+      <c r="E56">
+        <v>25</v>
+      </c>
+      <c r="F56">
+        <v>80</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>100</v>
+      </c>
+      <c r="E57">
+        <v>30</v>
+      </c>
+      <c r="F57">
+        <v>50</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>100</v>
+      </c>
+      <c r="E58">
+        <v>30</v>
+      </c>
+      <c r="F58">
+        <v>55</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="0"/>
+        <v>0.35064935064935066</v>
+      </c>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>100</v>
+      </c>
+      <c r="E59">
+        <v>30</v>
+      </c>
+      <c r="F59">
+        <v>60</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>100</v>
+      </c>
+      <c r="E60">
+        <v>30</v>
+      </c>
+      <c r="F60">
+        <v>65</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="0"/>
+        <v>0.23076923076923078</v>
+      </c>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>100</v>
+      </c>
+      <c r="E61">
+        <v>30</v>
+      </c>
+      <c r="F61">
+        <v>70</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="0"/>
+        <v>0.18367346938775511</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="E62">
+        <v>30</v>
+      </c>
+      <c r="F62">
+        <v>75</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>100</v>
+      </c>
+      <c r="E63">
+        <v>30</v>
+      </c>
+      <c r="F63">
+        <v>80</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="0"/>
+        <v>0.10714285714285714</v>
+      </c>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>100</v>
+      </c>
+      <c r="E64">
+        <v>35</v>
+      </c>
+      <c r="F64">
+        <v>55</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="0"/>
+        <v>0.44055944055944057</v>
+      </c>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>100</v>
+      </c>
+      <c r="E65">
+        <v>35</v>
+      </c>
+      <c r="F65">
+        <v>60</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="0"/>
+        <v>0.35897435897435898</v>
+      </c>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>100</v>
+      </c>
+      <c r="E66">
+        <v>35</v>
+      </c>
+      <c r="F66">
+        <v>65</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="0"/>
+        <v>0.28994082840236685</v>
+      </c>
+    </row>
+    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>100</v>
+      </c>
+      <c r="E67">
+        <v>35</v>
+      </c>
+      <c r="F67">
+        <v>70</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="0"/>
+        <v>0.23076923076923078</v>
+      </c>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>100</v>
+      </c>
+      <c r="E68">
+        <v>35</v>
+      </c>
+      <c r="F68">
+        <v>75</v>
+      </c>
+      <c r="I68">
+        <f t="shared" ref="I68:I84" si="10">E68*(D68-F68)/((D68-E68)*F68)</f>
+        <v>0.17948717948717949</v>
+      </c>
+    </row>
+    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>100</v>
+      </c>
+      <c r="E69">
+        <v>35</v>
+      </c>
+      <c r="F69">
+        <v>80</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="10"/>
+        <v>0.13461538461538461</v>
+      </c>
+    </row>
+    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>100</v>
+      </c>
+      <c r="E70">
+        <v>40</v>
+      </c>
+      <c r="F70">
+        <v>60</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="10"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>100</v>
+      </c>
+      <c r="E71">
+        <v>40</v>
+      </c>
+      <c r="F71">
+        <v>65</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="10"/>
+        <v>0.35897435897435898</v>
+      </c>
+    </row>
+    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>100</v>
+      </c>
+      <c r="E72">
+        <v>40</v>
+      </c>
+      <c r="F72">
+        <v>70</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="10"/>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>100</v>
+      </c>
+      <c r="E73">
+        <v>40</v>
+      </c>
+      <c r="F73">
+        <v>75</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="10"/>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>100</v>
+      </c>
+      <c r="E74">
+        <v>40</v>
+      </c>
+      <c r="F74">
+        <v>80</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>100</v>
+      </c>
+      <c r="E75">
+        <v>45</v>
+      </c>
+      <c r="F75">
+        <v>65</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="10"/>
+        <v>0.44055944055944057</v>
+      </c>
+    </row>
+    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>100</v>
+      </c>
+      <c r="E76">
+        <v>45</v>
+      </c>
+      <c r="F76">
+        <v>70</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="10"/>
+        <v>0.35064935064935066</v>
+      </c>
+    </row>
+    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>100</v>
+      </c>
+      <c r="E77">
+        <v>45</v>
+      </c>
+      <c r="F77">
+        <v>75</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="10"/>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>100</v>
+      </c>
+      <c r="E78">
+        <v>45</v>
+      </c>
+      <c r="F78">
+        <v>80</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="10"/>
+        <v>0.20454545454545456</v>
+      </c>
+    </row>
+    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>100</v>
+      </c>
+      <c r="E79">
+        <v>50</v>
+      </c>
+      <c r="F79">
+        <v>70</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="10"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>100</v>
+      </c>
+      <c r="E80">
+        <v>50</v>
+      </c>
+      <c r="F80">
+        <v>75</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="10"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>100</v>
+      </c>
+      <c r="E81">
+        <v>50</v>
+      </c>
+      <c r="F81">
+        <v>80</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>100</v>
+      </c>
+      <c r="E82">
+        <v>55</v>
+      </c>
+      <c r="F82">
+        <v>75</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="10"/>
+        <v>0.40740740740740738</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>100</v>
+      </c>
+      <c r="E83">
+        <v>55</v>
+      </c>
+      <c r="F83">
+        <v>80</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="10"/>
+        <v>0.30555555555555558</v>
+      </c>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>100</v>
+      </c>
+      <c r="E84">
+        <v>60</v>
+      </c>
+      <c r="F84">
+        <v>80</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="10"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N88" t="s">
+        <v>15</v>
+      </c>
+      <c r="O88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89">
+        <v>34</v>
+      </c>
+      <c r="D89">
+        <v>100</v>
+      </c>
+      <c r="E89">
+        <v>40</v>
+      </c>
+      <c r="F89">
+        <v>60</v>
+      </c>
+      <c r="G89">
+        <v>25</v>
+      </c>
+      <c r="H89">
+        <v>45</v>
+      </c>
+      <c r="I89">
+        <f t="shared" ref="I89" si="11">E89*(D89-F89)/((D89-E89)*F89)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J89">
+        <f t="shared" ref="J89" si="12">G89*(D89-H89)/((D89-G89)*H89)</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="K89">
+        <f t="shared" ref="K89" si="13">I89/J89</f>
+        <v>1.0909090909090908</v>
+      </c>
+      <c r="L89">
+        <f t="shared" ref="L89" si="14">ABS(K89-1)</f>
+        <v>9.0909090909090828E-2</v>
+      </c>
+      <c r="M89" t="b">
+        <f t="shared" ref="M89" si="15">NOT(OR(K89&lt;1,L89&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>35</v>
+      </c>
+      <c r="D90">
+        <v>100</v>
+      </c>
+      <c r="E90">
+        <v>40</v>
+      </c>
+      <c r="F90">
+        <v>60</v>
+      </c>
+      <c r="G90">
+        <v>30</v>
+      </c>
+      <c r="H90">
+        <v>55</v>
+      </c>
+      <c r="I90">
+        <f t="shared" ref="I90" si="16">E90*(D90-F90)/((D90-E90)*F90)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J90">
+        <f t="shared" ref="J90" si="17">G90*(D90-H90)/((D90-G90)*H90)</f>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="K90">
+        <f t="shared" ref="K90" si="18">I90/J90</f>
+        <v>1.2674897119341564</v>
+      </c>
+      <c r="L90">
+        <f t="shared" ref="L90" si="19">ABS(K90-1)</f>
+        <v>0.26748971193415638</v>
+      </c>
+      <c r="M90" t="b">
+        <f t="shared" ref="M90" si="20">NOT(OR(K90&lt;1,L90&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>36</v>
+      </c>
+      <c r="D91">
+        <v>100</v>
+      </c>
+      <c r="E91">
+        <v>40</v>
+      </c>
+      <c r="F91">
+        <v>60</v>
+      </c>
+      <c r="G91">
+        <v>35</v>
+      </c>
+      <c r="H91">
+        <v>60</v>
+      </c>
+      <c r="I91">
+        <f t="shared" ref="I91" si="21">E91*(D91-F91)/((D91-E91)*F91)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J91">
+        <f t="shared" ref="J91" si="22">G91*(D91-H91)/((D91-G91)*H91)</f>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="K91">
+        <f t="shared" ref="K91" si="23">I91/J91</f>
+        <v>1.2380952380952379</v>
+      </c>
+      <c r="L91">
+        <f t="shared" ref="L91" si="24">ABS(K91-1)</f>
+        <v>0.23809523809523792</v>
+      </c>
+      <c r="M91" t="b">
+        <f t="shared" ref="M91" si="25">NOT(OR(K91&lt;1,L91&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="N91" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>37</v>
+      </c>
+      <c r="D92">
+        <v>100</v>
+      </c>
+      <c r="E92">
+        <v>40</v>
+      </c>
+      <c r="F92">
+        <v>60</v>
+      </c>
+      <c r="G92">
+        <v>20</v>
+      </c>
+      <c r="H92">
+        <v>45</v>
+      </c>
+      <c r="I92">
+        <f t="shared" ref="I92:I98" si="26">E92*(D92-F92)/((D92-E92)*F92)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J92">
+        <f t="shared" ref="J92:J98" si="27">G92*(D92-H92)/((D92-G92)*H92)</f>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="K92">
+        <f t="shared" ref="K92:K98" si="28">I92/J92</f>
+        <v>1.4545454545454544</v>
+      </c>
+      <c r="L92">
+        <f t="shared" ref="L92:L98" si="29">ABS(K92-1)</f>
+        <v>0.45454545454545436</v>
+      </c>
+      <c r="M92" t="b">
+        <f t="shared" ref="M92:M98" si="30">NOT(OR(K92&lt;1,L92&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>38</v>
+      </c>
+      <c r="D93">
+        <v>100</v>
+      </c>
+      <c r="E93">
+        <v>40</v>
+      </c>
+      <c r="F93">
+        <v>60</v>
+      </c>
+      <c r="G93">
+        <v>20</v>
+      </c>
+      <c r="H93">
+        <v>50</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="26"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="27"/>
+        <v>0.25</v>
+      </c>
+      <c r="K93">
+        <f t="shared" si="28"/>
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="29"/>
+        <v>0.77777777777777768</v>
+      </c>
+      <c r="M93" t="b">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="N93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>39</v>
+      </c>
+      <c r="D94">
+        <v>100</v>
+      </c>
+      <c r="E94">
+        <v>40</v>
+      </c>
+      <c r="F94">
+        <v>60</v>
+      </c>
+      <c r="G94">
+        <v>20</v>
+      </c>
+      <c r="H94">
+        <v>55</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="26"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="27"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="28"/>
+        <v>2.1728395061728394</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="29"/>
+        <v>1.1728395061728394</v>
+      </c>
+      <c r="M94" t="b">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>40</v>
+      </c>
+      <c r="D95">
+        <v>100</v>
+      </c>
+      <c r="E95">
+        <v>40</v>
+      </c>
+      <c r="F95">
+        <v>60</v>
+      </c>
+      <c r="G95">
+        <v>25</v>
+      </c>
+      <c r="H95">
+        <v>70</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="26"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="27"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="28"/>
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="29"/>
+        <v>2.1111111111111112</v>
+      </c>
+      <c r="M95" t="b">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>41</v>
+      </c>
+      <c r="D96">
+        <v>100</v>
+      </c>
+      <c r="E96">
+        <v>40</v>
+      </c>
+      <c r="F96">
+        <v>60</v>
+      </c>
+      <c r="G96">
+        <v>25</v>
+      </c>
+      <c r="H96">
+        <v>75</v>
+      </c>
+      <c r="I96">
+        <f t="shared" ref="I96" si="31">E96*(D96-F96)/((D96-E96)*F96)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J96">
+        <f t="shared" ref="J96" si="32">G96*(D96-H96)/((D96-G96)*H96)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K96">
+        <f t="shared" ref="K96" si="33">I96/J96</f>
+        <v>4</v>
+      </c>
+      <c r="L96">
+        <f t="shared" ref="L96" si="34">ABS(K96-1)</f>
+        <v>3</v>
+      </c>
+      <c r="M96" t="b">
+        <f t="shared" ref="M96" si="35">NOT(OR(K96&lt;1,L96&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>42</v>
+      </c>
+      <c r="D97">
+        <v>100</v>
+      </c>
+      <c r="E97">
+        <v>40</v>
+      </c>
+      <c r="F97">
+        <v>60</v>
+      </c>
+      <c r="G97">
+        <v>30</v>
+      </c>
+      <c r="H97">
+        <v>80</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="26"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="27"/>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="28"/>
+        <v>4.1481481481481479</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="29"/>
+        <v>3.1481481481481479</v>
+      </c>
+      <c r="M97" t="b">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>43</v>
+      </c>
+      <c r="D98">
+        <v>100</v>
+      </c>
+      <c r="E98">
+        <v>40</v>
+      </c>
+      <c r="F98">
+        <v>60</v>
+      </c>
+      <c r="G98">
+        <v>20</v>
+      </c>
+      <c r="H98">
+        <v>80</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="26"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="27"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K98">
+        <f t="shared" si="28"/>
+        <v>7.1111111111111107</v>
+      </c>
+      <c r="L98">
+        <f t="shared" si="29"/>
+        <v>6.1111111111111107</v>
+      </c>
+      <c r="M98" t="b">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="N98" t="s">
+        <v>13</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>44</v>
+      </c>
+      <c r="D99">
+        <v>100</v>
+      </c>
+      <c r="E99">
+        <v>25</v>
+      </c>
+      <c r="F99">
+        <v>45</v>
+      </c>
+      <c r="G99">
+        <v>30</v>
+      </c>
+      <c r="H99">
+        <v>55</v>
+      </c>
+      <c r="I99">
+        <f>E99*(D99-F99)/((D99-E99)*F99)</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J99">
+        <f>G99*(D99-H99)/((D99-G99)*H99)</f>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="K99">
+        <f>I99/J99</f>
+        <v>1.1618655692729767</v>
+      </c>
+      <c r="L99">
+        <f>ABS(K99-1)</f>
+        <v>0.16186556927297668</v>
+      </c>
+      <c r="M99" t="b">
+        <f>NOT(OR(K99&lt;1,L99&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>45</v>
+      </c>
+      <c r="D100">
+        <v>100</v>
+      </c>
+      <c r="E100">
+        <v>25</v>
+      </c>
+      <c r="F100">
+        <v>45</v>
+      </c>
+      <c r="G100">
+        <v>35</v>
+      </c>
+      <c r="H100">
+        <v>60</v>
+      </c>
+      <c r="I100">
+        <f>E100*(D100-F100)/((D100-E100)*F100)</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J100">
+        <f>G100*(D100-H100)/((D100-G100)*H100)</f>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="K100">
+        <f>I100/J100</f>
+        <v>1.1349206349206349</v>
+      </c>
+      <c r="L100">
+        <f>ABS(K100-1)</f>
+        <v>0.13492063492063489</v>
+      </c>
+      <c r="M100" t="b">
+        <f>NOT(OR(K100&lt;1,L100&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>46</v>
+      </c>
+      <c r="D101">
+        <v>100</v>
+      </c>
+      <c r="E101">
+        <v>25</v>
+      </c>
+      <c r="F101">
+        <v>45</v>
+      </c>
+      <c r="G101">
+        <v>20</v>
+      </c>
+      <c r="H101">
+        <v>45</v>
+      </c>
+      <c r="I101">
+        <f t="shared" ref="I101:I108" si="36">E101*(D101-F101)/((D101-E101)*F101)</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J101">
+        <f t="shared" ref="J101:J108" si="37">G101*(D101-H101)/((D101-G101)*H101)</f>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="K101">
+        <f t="shared" ref="K101:K108" si="38">I101/J101</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L101">
+        <f t="shared" ref="L101:L108" si="39">ABS(K101-1)</f>
+        <v>0.33333333333333326</v>
+      </c>
+      <c r="M101" t="b">
+        <f t="shared" ref="M101:M108" si="40">NOT(OR(K101&lt;1,L101&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>47</v>
+      </c>
+      <c r="D102">
+        <v>100</v>
+      </c>
+      <c r="E102">
+        <v>25</v>
+      </c>
+      <c r="F102">
+        <v>45</v>
+      </c>
+      <c r="G102">
+        <v>20</v>
+      </c>
+      <c r="H102">
+        <v>50</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="36"/>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="37"/>
+        <v>0.25</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="38"/>
+        <v>1.6296296296296295</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="39"/>
+        <v>0.62962962962962954</v>
+      </c>
+      <c r="M102" t="b">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>48</v>
+      </c>
+      <c r="D103">
+        <v>100</v>
+      </c>
+      <c r="E103">
+        <v>25</v>
+      </c>
+      <c r="F103">
+        <v>45</v>
+      </c>
+      <c r="G103">
+        <v>20</v>
+      </c>
+      <c r="H103">
+        <v>55</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="36"/>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="37"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="38"/>
+        <v>1.9917695473251027</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="39"/>
+        <v>0.9917695473251027</v>
+      </c>
+      <c r="M103" t="b">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="N103" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <v>49</v>
+      </c>
+      <c r="D104">
+        <v>100</v>
+      </c>
+      <c r="E104">
+        <v>25</v>
+      </c>
+      <c r="F104">
+        <v>45</v>
+      </c>
+      <c r="G104">
+        <v>25</v>
+      </c>
+      <c r="H104">
+        <v>70</v>
+      </c>
+      <c r="I104">
+        <f t="shared" si="36"/>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J104">
+        <f t="shared" si="37"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K104">
+        <f t="shared" si="38"/>
+        <v>2.8518518518518516</v>
+      </c>
+      <c r="L104">
+        <f t="shared" si="39"/>
+        <v>1.8518518518518516</v>
+      </c>
+      <c r="M104" t="b">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>50</v>
+      </c>
+      <c r="D105">
+        <v>100</v>
+      </c>
+      <c r="E105">
+        <v>25</v>
+      </c>
+      <c r="F105">
+        <v>45</v>
+      </c>
+      <c r="G105">
+        <v>25</v>
+      </c>
+      <c r="H105">
+        <v>75</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="36"/>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="37"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K105">
+        <f t="shared" si="38"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="L105">
+        <f t="shared" si="39"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="M105" t="b">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <v>51</v>
+      </c>
+      <c r="D106">
+        <v>100</v>
+      </c>
+      <c r="E106">
+        <v>25</v>
+      </c>
+      <c r="F106">
+        <v>45</v>
+      </c>
+      <c r="G106">
+        <v>30</v>
+      </c>
+      <c r="H106">
+        <v>80</v>
+      </c>
+      <c r="I106">
+        <f t="shared" ref="I106" si="41">E106*(D106-F106)/((D106-E106)*F106)</f>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J106">
+        <f t="shared" ref="J106" si="42">G106*(D106-H106)/((D106-G106)*H106)</f>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="K106">
+        <f t="shared" ref="K106" si="43">I106/J106</f>
+        <v>3.8024691358024691</v>
+      </c>
+      <c r="L106">
+        <f t="shared" ref="L106" si="44">ABS(K106-1)</f>
+        <v>2.8024691358024691</v>
+      </c>
+      <c r="M106" t="b">
+        <f t="shared" ref="M106" si="45">NOT(OR(K106&lt;1,L106&lt;0.05))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <v>52</v>
+      </c>
+      <c r="D107">
+        <v>100</v>
+      </c>
+      <c r="E107">
+        <v>25</v>
+      </c>
+      <c r="F107">
+        <v>45</v>
+      </c>
+      <c r="G107">
+        <v>20</v>
+      </c>
+      <c r="H107">
+        <v>80</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="36"/>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="37"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K107">
+        <f t="shared" si="38"/>
+        <v>6.5185185185185182</v>
+      </c>
+      <c r="L107">
+        <f t="shared" si="39"/>
+        <v>5.5185185185185182</v>
+      </c>
+      <c r="M107" t="b">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <v>53</v>
+      </c>
+      <c r="D108">
+        <v>100</v>
+      </c>
+      <c r="E108">
+        <v>30</v>
+      </c>
+      <c r="F108">
+        <v>55</v>
+      </c>
+      <c r="G108">
+        <v>20</v>
+      </c>
+      <c r="H108">
+        <v>45</v>
+      </c>
+      <c r="I108">
+        <f t="shared" si="36"/>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="37"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="K108">
+        <f t="shared" si="38"/>
+        <v>1.1475796930342383</v>
+      </c>
+      <c r="L108">
+        <f t="shared" si="39"/>
+        <v>0.14757969303423835</v>
+      </c>
+      <c r="M108" t="b">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <v>54</v>
+      </c>
+      <c r="D109">
+        <v>100</v>
+      </c>
+      <c r="E109">
+        <v>30</v>
+      </c>
+      <c r="F109">
+        <v>55</v>
+      </c>
+      <c r="G109">
+        <v>20</v>
+      </c>
+      <c r="H109">
+        <v>50</v>
+      </c>
+      <c r="I109">
+        <f t="shared" ref="I109:I128" si="46">E109*(D109-F109)/((D109-E109)*F109)</f>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="J109">
+        <f t="shared" ref="J109:J128" si="47">G109*(D109-H109)/((D109-G109)*H109)</f>
+        <v>0.25</v>
+      </c>
+      <c r="K109">
+        <f t="shared" ref="K109:K128" si="48">I109/J109</f>
+        <v>1.4025974025974026</v>
+      </c>
+      <c r="L109">
+        <f t="shared" ref="L109:L128" si="49">ABS(K109-1)</f>
+        <v>0.40259740259740262</v>
+      </c>
+      <c r="M109" t="b">
+        <f t="shared" ref="M109:M128" si="50">NOT(OR(K109&lt;1,L109&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="N109" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <v>55</v>
+      </c>
+      <c r="D110">
+        <v>100</v>
+      </c>
+      <c r="E110">
+        <v>30</v>
+      </c>
+      <c r="F110">
+        <v>55</v>
+      </c>
+      <c r="G110">
+        <v>20</v>
+      </c>
+      <c r="H110">
+        <v>55</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="46"/>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="47"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="48"/>
+        <v>1.7142857142857142</v>
+      </c>
+      <c r="L110">
+        <f t="shared" si="49"/>
+        <v>0.71428571428571419</v>
+      </c>
+      <c r="M110" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <v>56</v>
+      </c>
+      <c r="D111">
+        <v>100</v>
+      </c>
+      <c r="E111">
+        <v>30</v>
+      </c>
+      <c r="F111">
+        <v>55</v>
+      </c>
+      <c r="G111">
+        <v>25</v>
+      </c>
+      <c r="H111">
+        <v>70</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="46"/>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="47"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="48"/>
+        <v>2.4545454545454546</v>
+      </c>
+      <c r="L111">
+        <f t="shared" si="49"/>
+        <v>1.4545454545454546</v>
+      </c>
+      <c r="M111" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="N111" t="s">
+        <v>13</v>
+      </c>
+      <c r="O111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <v>57</v>
+      </c>
+      <c r="D112">
+        <v>100</v>
+      </c>
+      <c r="E112">
+        <v>30</v>
+      </c>
+      <c r="F112">
+        <v>55</v>
+      </c>
+      <c r="G112">
+        <v>25</v>
+      </c>
+      <c r="H112">
+        <v>75</v>
+      </c>
+      <c r="I112">
+        <f t="shared" si="46"/>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="47"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K112">
+        <f t="shared" si="48"/>
+        <v>3.1558441558441559</v>
+      </c>
+      <c r="L112">
+        <f t="shared" si="49"/>
+        <v>2.1558441558441559</v>
+      </c>
+      <c r="M112" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <v>58</v>
+      </c>
+      <c r="D113">
+        <v>100</v>
+      </c>
+      <c r="E113">
+        <v>30</v>
+      </c>
+      <c r="F113">
+        <v>55</v>
+      </c>
+      <c r="G113">
+        <v>20</v>
+      </c>
+      <c r="H113">
+        <v>80</v>
+      </c>
+      <c r="I113">
+        <f t="shared" si="46"/>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="47"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K113">
+        <f t="shared" si="48"/>
+        <v>5.6103896103896105</v>
+      </c>
+      <c r="L113">
+        <f t="shared" si="49"/>
+        <v>4.6103896103896105</v>
+      </c>
+      <c r="M113" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <v>59</v>
+      </c>
+      <c r="D114">
+        <v>100</v>
+      </c>
+      <c r="E114">
+        <v>20</v>
+      </c>
+      <c r="F114">
+        <v>45</v>
+      </c>
+      <c r="G114">
+        <v>20</v>
+      </c>
+      <c r="H114">
+        <v>50</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="46"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="47"/>
+        <v>0.25</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="48"/>
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="L114">
+        <f t="shared" si="49"/>
+        <v>0.22222222222222232</v>
+      </c>
+      <c r="M114" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="O114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <v>60</v>
+      </c>
+      <c r="D115">
+        <v>100</v>
+      </c>
+      <c r="E115">
+        <v>20</v>
+      </c>
+      <c r="F115">
+        <v>45</v>
+      </c>
+      <c r="G115">
+        <v>20</v>
+      </c>
+      <c r="H115">
+        <v>55</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="46"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="J115">
+        <f t="shared" si="47"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="K115">
+        <f t="shared" si="48"/>
+        <v>1.4938271604938271</v>
+      </c>
+      <c r="L115">
+        <f t="shared" si="49"/>
+        <v>0.49382716049382713</v>
+      </c>
+      <c r="M115" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="N115" t="s">
+        <v>13</v>
+      </c>
+      <c r="O115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>61</v>
+      </c>
+      <c r="D116">
+        <v>100</v>
+      </c>
+      <c r="E116">
+        <v>20</v>
+      </c>
+      <c r="F116">
+        <v>45</v>
+      </c>
+      <c r="G116">
+        <v>25</v>
+      </c>
+      <c r="H116">
+        <v>70</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="46"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="47"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K116">
+        <f t="shared" si="48"/>
+        <v>2.1388888888888893</v>
+      </c>
+      <c r="L116">
+        <f t="shared" si="49"/>
+        <v>1.1388888888888893</v>
+      </c>
+      <c r="M116" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <v>62</v>
+      </c>
+      <c r="D117">
+        <v>100</v>
+      </c>
+      <c r="E117">
+        <v>20</v>
+      </c>
+      <c r="F117">
+        <v>45</v>
+      </c>
+      <c r="G117">
+        <v>25</v>
+      </c>
+      <c r="H117">
+        <v>75</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="46"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="47"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K117">
+        <f t="shared" si="48"/>
+        <v>2.7500000000000004</v>
+      </c>
+      <c r="L117">
+        <f t="shared" si="49"/>
+        <v>1.7500000000000004</v>
+      </c>
+      <c r="M117" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <v>63</v>
+      </c>
+      <c r="D118">
+        <v>100</v>
+      </c>
+      <c r="E118">
+        <v>20</v>
+      </c>
+      <c r="F118">
+        <v>45</v>
+      </c>
+      <c r="G118">
+        <v>20</v>
+      </c>
+      <c r="H118">
+        <v>80</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="46"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="47"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K118">
+        <f t="shared" si="48"/>
+        <v>4.8888888888888893</v>
+      </c>
+      <c r="L118">
+        <f t="shared" si="49"/>
+        <v>3.8888888888888893</v>
+      </c>
+      <c r="M118" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="N118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <v>64</v>
+      </c>
+      <c r="D119">
+        <v>100</v>
+      </c>
+      <c r="E119">
+        <v>20</v>
+      </c>
+      <c r="F119">
+        <v>50</v>
+      </c>
+      <c r="G119">
+        <v>20</v>
+      </c>
+      <c r="H119">
+        <v>55</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="46"/>
+        <v>0.25</v>
+      </c>
+      <c r="J119">
+        <f t="shared" si="47"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="K119">
+        <f t="shared" si="48"/>
+        <v>1.2222222222222221</v>
+      </c>
+      <c r="L119">
+        <f t="shared" si="49"/>
+        <v>0.2222222222222221</v>
+      </c>
+      <c r="M119" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="O119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <v>65</v>
+      </c>
+      <c r="D120">
+        <v>100</v>
+      </c>
+      <c r="E120">
+        <v>20</v>
+      </c>
+      <c r="F120">
+        <v>50</v>
+      </c>
+      <c r="G120">
+        <v>25</v>
+      </c>
+      <c r="H120">
+        <v>70</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="46"/>
+        <v>0.25</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="47"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="48"/>
+        <v>1.75</v>
+      </c>
+      <c r="L120">
+        <f t="shared" si="49"/>
+        <v>0.75</v>
+      </c>
+      <c r="M120" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <v>66</v>
+      </c>
+      <c r="D121">
+        <v>100</v>
+      </c>
+      <c r="E121">
+        <v>20</v>
+      </c>
+      <c r="F121">
+        <v>50</v>
+      </c>
+      <c r="G121">
+        <v>25</v>
+      </c>
+      <c r="H121">
+        <v>75</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="46"/>
+        <v>0.25</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="47"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K121">
+        <f t="shared" si="48"/>
+        <v>2.25</v>
+      </c>
+      <c r="L121">
+        <f t="shared" si="49"/>
+        <v>1.25</v>
+      </c>
+      <c r="M121" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="N121" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <v>67</v>
+      </c>
+      <c r="D122">
+        <v>100</v>
+      </c>
+      <c r="E122">
+        <v>20</v>
+      </c>
+      <c r="F122">
+        <v>50</v>
+      </c>
+      <c r="G122">
+        <v>20</v>
+      </c>
+      <c r="H122">
+        <v>80</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="46"/>
+        <v>0.25</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="47"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K122">
+        <f t="shared" si="48"/>
+        <v>4</v>
+      </c>
+      <c r="L122">
+        <f t="shared" si="49"/>
+        <v>3</v>
+      </c>
+      <c r="M122" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <v>68</v>
+      </c>
+      <c r="D123">
+        <v>100</v>
+      </c>
+      <c r="E123">
+        <v>20</v>
+      </c>
+      <c r="F123">
+        <v>55</v>
+      </c>
+      <c r="G123">
+        <v>25</v>
+      </c>
+      <c r="H123">
+        <v>70</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="46"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="47"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K123">
+        <f t="shared" si="48"/>
+        <v>1.4318181818181819</v>
+      </c>
+      <c r="L123">
+        <f t="shared" si="49"/>
+        <v>0.43181818181818188</v>
+      </c>
+      <c r="M123" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="N123" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <v>69</v>
+      </c>
+      <c r="D124">
+        <v>100</v>
+      </c>
+      <c r="E124">
+        <v>20</v>
+      </c>
+      <c r="F124">
+        <v>55</v>
+      </c>
+      <c r="G124">
+        <v>25</v>
+      </c>
+      <c r="H124">
+        <v>75</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="46"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="47"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="48"/>
+        <v>1.8409090909090911</v>
+      </c>
+      <c r="L124">
+        <f t="shared" si="49"/>
+        <v>0.84090909090909105</v>
+      </c>
+      <c r="M124" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <v>70</v>
+      </c>
+      <c r="D125">
+        <v>100</v>
+      </c>
+      <c r="E125">
+        <v>20</v>
+      </c>
+      <c r="F125">
+        <v>55</v>
+      </c>
+      <c r="G125">
+        <v>20</v>
+      </c>
+      <c r="H125">
+        <v>80</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="46"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="J125">
+        <f t="shared" si="47"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K125">
+        <f t="shared" si="48"/>
+        <v>3.2727272727272729</v>
+      </c>
+      <c r="L125">
+        <f t="shared" si="49"/>
+        <v>2.2727272727272729</v>
+      </c>
+      <c r="M125" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>71</v>
+      </c>
+      <c r="D126">
+        <v>100</v>
+      </c>
+      <c r="E126">
+        <v>25</v>
+      </c>
+      <c r="F126">
+        <v>70</v>
+      </c>
+      <c r="G126">
+        <v>25</v>
+      </c>
+      <c r="H126">
+        <v>75</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="46"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J126">
+        <f t="shared" si="47"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="48"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="L126">
+        <f t="shared" si="49"/>
+        <v>0.28571428571428581</v>
+      </c>
+      <c r="M126" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <v>72</v>
+      </c>
+      <c r="D127">
+        <v>100</v>
+      </c>
+      <c r="E127">
+        <v>25</v>
+      </c>
+      <c r="F127">
+        <v>70</v>
+      </c>
+      <c r="G127">
+        <v>20</v>
+      </c>
+      <c r="H127">
+        <v>80</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="46"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J127">
+        <f t="shared" si="47"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="48"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="L127">
+        <f t="shared" si="49"/>
+        <v>1.2857142857142856</v>
+      </c>
+      <c r="M127" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="N127" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <v>73</v>
+      </c>
+      <c r="D128">
+        <v>100</v>
+      </c>
+      <c r="E128">
+        <v>25</v>
+      </c>
+      <c r="F128">
+        <v>75</v>
+      </c>
+      <c r="G128">
+        <v>20</v>
+      </c>
+      <c r="H128">
+        <v>80</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="46"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J128">
+        <f t="shared" si="47"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K128">
+        <f t="shared" si="48"/>
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="L128">
+        <f t="shared" si="49"/>
+        <v>0.77777777777777768</v>
+      </c>
+      <c r="M128" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="W8:W37">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="lessThan">
+  <conditionalFormatting sqref="W8:W37 L89:L128">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V8:V37">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
+  <conditionalFormatting sqref="V8:V37 K89:K128">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N37">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2966,21 +5651,69 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K37">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L37">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M37">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="M4:M37 M89:M128">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>FALSE</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I40:I84">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:J37">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I89:I128">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J89:J128">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new tags with big differences in their cross ratios
</commit_message>
<xml_diff>
--- a/cob_fiducials/common/files/fiducials/pi/Fiducials.xlsx
+++ b/cob_fiducials/common/files/fiducials/pi/Fiducials.xlsx
@@ -105,287 +105,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -803,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W128"/>
+  <dimension ref="B2:W129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:XFD128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4808,27 +4528,24 @@
         <v>50</v>
       </c>
       <c r="I109">
-        <f t="shared" ref="I109:I128" si="46">E109*(D109-F109)/((D109-E109)*F109)</f>
+        <f t="shared" ref="I109:I129" si="46">E109*(D109-F109)/((D109-E109)*F109)</f>
         <v>0.35064935064935066</v>
       </c>
       <c r="J109">
-        <f t="shared" ref="J109:J128" si="47">G109*(D109-H109)/((D109-G109)*H109)</f>
+        <f t="shared" ref="J109:J129" si="47">G109*(D109-H109)/((D109-G109)*H109)</f>
         <v>0.25</v>
       </c>
       <c r="K109">
-        <f t="shared" ref="K109:K128" si="48">I109/J109</f>
+        <f t="shared" ref="K109:K129" si="48">I109/J109</f>
         <v>1.4025974025974026</v>
       </c>
       <c r="L109">
-        <f t="shared" ref="L109:L128" si="49">ABS(K109-1)</f>
+        <f t="shared" ref="L109:L129" si="49">ABS(K109-1)</f>
         <v>0.40259740259740262</v>
       </c>
       <c r="M109" t="b">
-        <f t="shared" ref="M109:M128" si="50">NOT(OR(K109&lt;1,L109&lt;0.05))</f>
-        <v>1</v>
-      </c>
-      <c r="N109" t="s">
-        <v>13</v>
+        <f t="shared" ref="M109:M129" si="50">NOT(OR(K109&lt;1,L109&lt;0.05))</f>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="3:15" x14ac:dyDescent="0.25">
@@ -4845,30 +4562,33 @@
         <v>55</v>
       </c>
       <c r="G110">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H110">
         <v>55</v>
       </c>
       <c r="I110">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="I110" si="51">E110*(D110-F110)/((D110-E110)*F110)</f>
         <v>0.35064935064935066</v>
       </c>
       <c r="J110">
-        <f t="shared" si="47"/>
-        <v>0.20454545454545456</v>
+        <f t="shared" ref="J110" si="52">G110*(D110-H110)/((D110-G110)*H110)</f>
+        <v>0.27272727272727271</v>
       </c>
       <c r="K110">
-        <f t="shared" si="48"/>
-        <v>1.7142857142857142</v>
+        <f t="shared" ref="K110" si="53">I110/J110</f>
+        <v>1.2857142857142858</v>
       </c>
       <c r="L110">
-        <f t="shared" si="49"/>
-        <v>0.71428571428571419</v>
+        <f t="shared" ref="L110" si="54">ABS(K110-1)</f>
+        <v>0.28571428571428581</v>
       </c>
       <c r="M110" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
+        <f t="shared" ref="M110" si="55">NOT(OR(K110&lt;1,L110&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="N110" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="3:15" x14ac:dyDescent="0.25">
@@ -4885,10 +4605,10 @@
         <v>55</v>
       </c>
       <c r="G111">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H111">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I111">
         <f t="shared" si="46"/>
@@ -4896,24 +4616,18 @@
       </c>
       <c r="J111">
         <f t="shared" si="47"/>
-        <v>0.14285714285714285</v>
+        <v>0.20454545454545456</v>
       </c>
       <c r="K111">
         <f t="shared" si="48"/>
-        <v>2.4545454545454546</v>
+        <v>1.7142857142857142</v>
       </c>
       <c r="L111">
         <f t="shared" si="49"/>
-        <v>1.4545454545454546</v>
+        <v>0.71428571428571419</v>
       </c>
       <c r="M111" t="b">
         <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-      <c r="N111" t="s">
-        <v>13</v>
-      </c>
-      <c r="O111">
         <v>1</v>
       </c>
     </row>
@@ -4934,7 +4648,7 @@
         <v>25</v>
       </c>
       <c r="H112">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I112">
         <f t="shared" si="46"/>
@@ -4942,18 +4656,24 @@
       </c>
       <c r="J112">
         <f t="shared" si="47"/>
-        <v>0.1111111111111111</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="K112">
         <f t="shared" si="48"/>
-        <v>3.1558441558441559</v>
+        <v>2.4545454545454546</v>
       </c>
       <c r="L112">
         <f t="shared" si="49"/>
-        <v>2.1558441558441559</v>
+        <v>1.4545454545454546</v>
       </c>
       <c r="M112" t="b">
         <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="N112" t="s">
+        <v>13</v>
+      </c>
+      <c r="O112">
         <v>1</v>
       </c>
     </row>
@@ -4971,10 +4691,10 @@
         <v>55</v>
       </c>
       <c r="G113">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H113">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I113">
         <f t="shared" si="46"/>
@@ -4982,15 +4702,15 @@
       </c>
       <c r="J113">
         <f t="shared" si="47"/>
-        <v>6.25E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K113">
         <f t="shared" si="48"/>
-        <v>5.6103896103896105</v>
+        <v>3.1558441558441559</v>
       </c>
       <c r="L113">
         <f t="shared" si="49"/>
-        <v>4.6103896103896105</v>
+        <v>2.1558441558441559</v>
       </c>
       <c r="M113" t="b">
         <f t="shared" si="50"/>
@@ -5005,39 +4725,36 @@
         <v>100</v>
       </c>
       <c r="E114">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F114">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G114">
         <v>20</v>
       </c>
       <c r="H114">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="I114">
         <f t="shared" si="46"/>
-        <v>0.30555555555555558</v>
+        <v>0.35064935064935066</v>
       </c>
       <c r="J114">
         <f t="shared" si="47"/>
-        <v>0.25</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K114">
         <f t="shared" si="48"/>
-        <v>1.2222222222222223</v>
+        <v>5.6103896103896105</v>
       </c>
       <c r="L114">
         <f t="shared" si="49"/>
-        <v>0.22222222222222232</v>
+        <v>4.6103896103896105</v>
       </c>
       <c r="M114" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
-      </c>
-      <c r="O114">
-        <v>3</v>
       </c>
     </row>
     <row r="115" spans="3:15" x14ac:dyDescent="0.25">
@@ -5057,7 +4774,7 @@
         <v>20</v>
       </c>
       <c r="H115">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I115">
         <f t="shared" si="46"/>
@@ -5065,25 +4782,22 @@
       </c>
       <c r="J115">
         <f t="shared" si="47"/>
-        <v>0.20454545454545456</v>
+        <v>0.25</v>
       </c>
       <c r="K115">
         <f t="shared" si="48"/>
-        <v>1.4938271604938271</v>
+        <v>1.2222222222222223</v>
       </c>
       <c r="L115">
         <f t="shared" si="49"/>
-        <v>0.49382716049382713</v>
+        <v>0.22222222222222232</v>
       </c>
       <c r="M115" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
       </c>
-      <c r="N115" t="s">
-        <v>13</v>
-      </c>
       <c r="O115">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="3:15" x14ac:dyDescent="0.25">
@@ -5100,10 +4814,10 @@
         <v>45</v>
       </c>
       <c r="G116">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H116">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I116">
         <f t="shared" si="46"/>
@@ -5111,19 +4825,25 @@
       </c>
       <c r="J116">
         <f t="shared" si="47"/>
-        <v>0.14285714285714285</v>
+        <v>0.20454545454545456</v>
       </c>
       <c r="K116">
         <f t="shared" si="48"/>
-        <v>2.1388888888888893</v>
+        <v>1.4938271604938271</v>
       </c>
       <c r="L116">
         <f t="shared" si="49"/>
-        <v>1.1388888888888893</v>
+        <v>0.49382716049382713</v>
       </c>
       <c r="M116" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
+      </c>
+      <c r="N116" t="s">
+        <v>13</v>
+      </c>
+      <c r="O116">
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="3:15" x14ac:dyDescent="0.25">
@@ -5143,7 +4863,7 @@
         <v>25</v>
       </c>
       <c r="H117">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I117">
         <f t="shared" si="46"/>
@@ -5151,15 +4871,15 @@
       </c>
       <c r="J117">
         <f t="shared" si="47"/>
-        <v>0.1111111111111111</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="K117">
         <f t="shared" si="48"/>
-        <v>2.7500000000000004</v>
+        <v>2.1388888888888893</v>
       </c>
       <c r="L117">
         <f t="shared" si="49"/>
-        <v>1.7500000000000004</v>
+        <v>1.1388888888888893</v>
       </c>
       <c r="M117" t="b">
         <f t="shared" si="50"/>
@@ -5180,10 +4900,10 @@
         <v>45</v>
       </c>
       <c r="G118">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H118">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I118">
         <f t="shared" si="46"/>
@@ -5191,22 +4911,19 @@
       </c>
       <c r="J118">
         <f t="shared" si="47"/>
-        <v>6.25E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K118">
         <f t="shared" si="48"/>
-        <v>4.8888888888888893</v>
+        <v>2.7500000000000004</v>
       </c>
       <c r="L118">
         <f t="shared" si="49"/>
-        <v>3.8888888888888893</v>
+        <v>1.7500000000000004</v>
       </c>
       <c r="M118" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
-      </c>
-      <c r="N118" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="119" spans="3:15" x14ac:dyDescent="0.25">
@@ -5220,36 +4937,36 @@
         <v>20</v>
       </c>
       <c r="F119">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G119">
         <v>20</v>
       </c>
       <c r="H119">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="I119">
         <f t="shared" si="46"/>
-        <v>0.25</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="J119">
         <f t="shared" si="47"/>
-        <v>0.20454545454545456</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K119">
         <f t="shared" si="48"/>
-        <v>1.2222222222222221</v>
+        <v>4.8888888888888893</v>
       </c>
       <c r="L119">
         <f t="shared" si="49"/>
-        <v>0.2222222222222221</v>
+        <v>3.8888888888888893</v>
       </c>
       <c r="M119" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
       </c>
-      <c r="O119">
-        <v>3</v>
+      <c r="N119" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="120" spans="3:15" x14ac:dyDescent="0.25">
@@ -5266,10 +4983,10 @@
         <v>50</v>
       </c>
       <c r="G120">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H120">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I120">
         <f t="shared" si="46"/>
@@ -5277,19 +4994,22 @@
       </c>
       <c r="J120">
         <f t="shared" si="47"/>
-        <v>0.14285714285714285</v>
+        <v>0.20454545454545456</v>
       </c>
       <c r="K120">
         <f t="shared" si="48"/>
-        <v>1.75</v>
+        <v>1.2222222222222221</v>
       </c>
       <c r="L120">
         <f t="shared" si="49"/>
-        <v>0.75</v>
+        <v>0.2222222222222221</v>
       </c>
       <c r="M120" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
+      </c>
+      <c r="O120">
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="3:15" x14ac:dyDescent="0.25">
@@ -5309,7 +5029,7 @@
         <v>25</v>
       </c>
       <c r="H121">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I121">
         <f t="shared" si="46"/>
@@ -5317,22 +5037,19 @@
       </c>
       <c r="J121">
         <f t="shared" si="47"/>
-        <v>0.1111111111111111</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="K121">
         <f t="shared" si="48"/>
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="L121">
         <f t="shared" si="49"/>
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="M121" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
-      </c>
-      <c r="N121" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="122" spans="3:15" x14ac:dyDescent="0.25">
@@ -5349,10 +5066,10 @@
         <v>50</v>
       </c>
       <c r="G122">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H122">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I122">
         <f t="shared" si="46"/>
@@ -5360,19 +5077,22 @@
       </c>
       <c r="J122">
         <f t="shared" si="47"/>
-        <v>6.25E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K122">
         <f t="shared" si="48"/>
-        <v>4</v>
+        <v>2.25</v>
       </c>
       <c r="L122">
         <f t="shared" si="49"/>
-        <v>3</v>
+        <v>1.25</v>
       </c>
       <c r="M122" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
+      </c>
+      <c r="N122" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="3:15" x14ac:dyDescent="0.25">
@@ -5386,36 +5106,33 @@
         <v>20</v>
       </c>
       <c r="F123">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G123">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H123">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I123">
         <f t="shared" si="46"/>
-        <v>0.20454545454545456</v>
+        <v>0.25</v>
       </c>
       <c r="J123">
         <f t="shared" si="47"/>
-        <v>0.14285714285714285</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K123">
         <f t="shared" si="48"/>
-        <v>1.4318181818181819</v>
+        <v>4</v>
       </c>
       <c r="L123">
         <f t="shared" si="49"/>
-        <v>0.43181818181818188</v>
+        <v>3</v>
       </c>
       <c r="M123" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
-      </c>
-      <c r="N123" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="124" spans="3:15" x14ac:dyDescent="0.25">
@@ -5435,7 +5152,7 @@
         <v>25</v>
       </c>
       <c r="H124">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I124">
         <f t="shared" si="46"/>
@@ -5443,19 +5160,22 @@
       </c>
       <c r="J124">
         <f t="shared" si="47"/>
-        <v>0.1111111111111111</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="K124">
         <f t="shared" si="48"/>
-        <v>1.8409090909090911</v>
+        <v>1.4318181818181819</v>
       </c>
       <c r="L124">
         <f t="shared" si="49"/>
-        <v>0.84090909090909105</v>
+        <v>0.43181818181818188</v>
       </c>
       <c r="M124" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
+      </c>
+      <c r="N124" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="3:15" x14ac:dyDescent="0.25">
@@ -5472,10 +5192,10 @@
         <v>55</v>
       </c>
       <c r="G125">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H125">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I125">
         <f t="shared" si="46"/>
@@ -5483,15 +5203,15 @@
       </c>
       <c r="J125">
         <f t="shared" si="47"/>
-        <v>6.25E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K125">
         <f t="shared" si="48"/>
-        <v>3.2727272727272729</v>
+        <v>1.8409090909090911</v>
       </c>
       <c r="L125">
         <f t="shared" si="49"/>
-        <v>2.2727272727272729</v>
+        <v>0.84090909090909105</v>
       </c>
       <c r="M125" t="b">
         <f t="shared" si="50"/>
@@ -5506,32 +5226,32 @@
         <v>100</v>
       </c>
       <c r="E126">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F126">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G126">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H126">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I126">
         <f t="shared" si="46"/>
-        <v>0.14285714285714285</v>
+        <v>0.20454545454545456</v>
       </c>
       <c r="J126">
         <f t="shared" si="47"/>
-        <v>0.1111111111111111</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K126">
         <f t="shared" si="48"/>
-        <v>1.2857142857142858</v>
+        <v>3.2727272727272729</v>
       </c>
       <c r="L126">
         <f t="shared" si="49"/>
-        <v>0.28571428571428581</v>
+        <v>2.2727272727272729</v>
       </c>
       <c r="M126" t="b">
         <f t="shared" si="50"/>
@@ -5552,10 +5272,10 @@
         <v>70</v>
       </c>
       <c r="G127">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H127">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I127">
         <f t="shared" si="46"/>
@@ -5563,22 +5283,19 @@
       </c>
       <c r="J127">
         <f t="shared" si="47"/>
-        <v>6.25E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K127">
         <f t="shared" si="48"/>
-        <v>2.2857142857142856</v>
+        <v>1.2857142857142858</v>
       </c>
       <c r="L127">
         <f t="shared" si="49"/>
-        <v>1.2857142857142856</v>
+        <v>0.28571428571428581</v>
       </c>
       <c r="M127" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
-      </c>
-      <c r="N127" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="128" spans="3:15" x14ac:dyDescent="0.25">
@@ -5592,7 +5309,7 @@
         <v>25</v>
       </c>
       <c r="F128">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G128">
         <v>20</v>
@@ -5602,7 +5319,7 @@
       </c>
       <c r="I128">
         <f t="shared" si="46"/>
-        <v>0.1111111111111111</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="J128">
         <f t="shared" si="47"/>
@@ -5610,24 +5327,67 @@
       </c>
       <c r="K128">
         <f t="shared" si="48"/>
-        <v>1.7777777777777777</v>
+        <v>2.2857142857142856</v>
       </c>
       <c r="L128">
         <f t="shared" si="49"/>
-        <v>0.77777777777777768</v>
+        <v>1.2857142857142856</v>
       </c>
       <c r="M128" t="b">
         <f t="shared" si="50"/>
         <v>1</v>
       </c>
+      <c r="N128" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <v>74</v>
+      </c>
+      <c r="D129">
+        <v>100</v>
+      </c>
+      <c r="E129">
+        <v>25</v>
+      </c>
+      <c r="F129">
+        <v>75</v>
+      </c>
+      <c r="G129">
+        <v>20</v>
+      </c>
+      <c r="H129">
+        <v>80</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="46"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J129">
+        <f t="shared" si="47"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="K129">
+        <f t="shared" si="48"/>
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="L129">
+        <f t="shared" si="49"/>
+        <v>0.77777777777777768</v>
+      </c>
+      <c r="M129" t="b">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="W8:W37 L89:L128">
+  <conditionalFormatting sqref="W8:W37 L89:L129">
     <cfRule type="cellIs" dxfId="11" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V8:V37 K89:K128">
+  <conditionalFormatting sqref="V8:V37 K89:K129">
     <cfRule type="cellIs" dxfId="10" priority="16" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -5660,7 +5420,7 @@
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M37 M89:M128">
+  <conditionalFormatting sqref="M4:M37 M89:M129">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
@@ -5692,7 +5452,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I89:I128">
+  <conditionalFormatting sqref="I89:I129">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -5704,7 +5464,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J89:J128">
+  <conditionalFormatting sqref="J89:J129">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
added 3 tags that are similar to (and therefore replacing) former 67, 69, 73 tags, but the new tags should have better visibility from far
</commit_message>
<xml_diff>
--- a/cob_fiducials/common/files/fiducials/pi/Fiducials.xlsx
+++ b/cob_fiducials/common/files/fiducials/pi/Fiducials.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Line 0 (y-axis)</t>
   </si>
@@ -65,6 +65,21 @@
   <si>
     <t>good distance to others</t>
   </si>
+  <si>
+    <t>has a 20mm edge (i.e. not good for long distance recognition)</t>
+  </si>
+  <si>
+    <t>~ 69</t>
+  </si>
+  <si>
+    <t>~ 63, 67</t>
+  </si>
+  <si>
+    <t>~ 79</t>
+  </si>
+  <si>
+    <t>~ 83</t>
+  </si>
 </sst>
 </file>
 
@@ -105,7 +120,27 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -153,6 +188,226 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -523,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W129"/>
+  <dimension ref="B2:W139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128:XFD128"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,6 +792,7 @@
     <col min="11" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.7109375" customWidth="1"/>
     <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:23" x14ac:dyDescent="0.25">
@@ -3003,6 +3259,9 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="J39" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
@@ -3021,6 +3280,10 @@
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
+      <c r="J40" t="b">
+        <f>OR(E40=20,F40=80,F40-E40=20)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D41">
@@ -3036,6 +3299,10 @@
         <f t="shared" si="0"/>
         <v>0.30555555555555558</v>
       </c>
+      <c r="J41" t="b">
+        <f t="shared" ref="J41:J84" si="10">OR(E41=20,F41=80,F41-E41=20)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D42">
@@ -3051,6 +3318,10 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
+      <c r="J42" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D43">
@@ -3066,6 +3337,10 @@
         <f t="shared" si="0"/>
         <v>0.20454545454545456</v>
       </c>
+      <c r="J43" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D44">
@@ -3081,6 +3356,10 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
+      <c r="J44" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D45">
@@ -3096,6 +3375,10 @@
         <f t="shared" si="0"/>
         <v>0.13461538461538461</v>
       </c>
+      <c r="J45" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D46">
@@ -3111,6 +3394,10 @@
         <f t="shared" si="0"/>
         <v>0.10714285714285714</v>
       </c>
+      <c r="J46" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D47">
@@ -3126,6 +3413,10 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
+      <c r="J47" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D48">
@@ -3141,8 +3432,12 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D49">
         <v>100</v>
       </c>
@@ -3156,8 +3451,12 @@
         <f t="shared" si="0"/>
         <v>0.40740740740740738</v>
       </c>
-    </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D50">
         <v>100</v>
       </c>
@@ -3171,8 +3470,12 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D51">
         <v>100</v>
       </c>
@@ -3186,8 +3489,12 @@
         <f t="shared" si="0"/>
         <v>0.27272727272727271</v>
       </c>
-    </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D52">
         <v>100</v>
       </c>
@@ -3201,8 +3508,12 @@
         <f t="shared" si="0"/>
         <v>0.22222222222222221</v>
       </c>
-    </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D53">
         <v>100</v>
       </c>
@@ -3216,8 +3527,12 @@
         <f t="shared" si="0"/>
         <v>0.17948717948717949</v>
       </c>
-    </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D54">
         <v>100</v>
       </c>
@@ -3231,8 +3546,12 @@
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-    </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>100</v>
       </c>
@@ -3246,8 +3565,12 @@
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D56">
         <v>100</v>
       </c>
@@ -3261,8 +3584,12 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>100</v>
       </c>
@@ -3276,8 +3603,12 @@
         <f t="shared" si="0"/>
         <v>0.42857142857142855</v>
       </c>
-    </row>
-    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D58">
         <v>100</v>
       </c>
@@ -3291,8 +3622,12 @@
         <f t="shared" si="0"/>
         <v>0.35064935064935066</v>
       </c>
-    </row>
-    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D59">
         <v>100</v>
       </c>
@@ -3306,8 +3641,12 @@
         <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
-    </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J59" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D60">
         <v>100</v>
       </c>
@@ -3321,8 +3660,12 @@
         <f t="shared" si="0"/>
         <v>0.23076923076923078</v>
       </c>
-    </row>
-    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J60" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D61">
         <v>100</v>
       </c>
@@ -3336,8 +3679,12 @@
         <f t="shared" si="0"/>
         <v>0.18367346938775511</v>
       </c>
-    </row>
-    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D62">
         <v>100</v>
       </c>
@@ -3351,8 +3698,12 @@
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
-    </row>
-    <row r="63" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D63">
         <v>100</v>
       </c>
@@ -3366,8 +3717,12 @@
         <f t="shared" si="0"/>
         <v>0.10714285714285714</v>
       </c>
-    </row>
-    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D64">
         <v>100</v>
       </c>
@@ -3381,8 +3736,12 @@
         <f t="shared" si="0"/>
         <v>0.44055944055944057</v>
       </c>
-    </row>
-    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>100</v>
       </c>
@@ -3396,8 +3755,12 @@
         <f t="shared" si="0"/>
         <v>0.35897435897435898</v>
       </c>
-    </row>
-    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J65" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D66">
         <v>100</v>
       </c>
@@ -3411,8 +3774,12 @@
         <f t="shared" si="0"/>
         <v>0.28994082840236685</v>
       </c>
-    </row>
-    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J66" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D67">
         <v>100</v>
       </c>
@@ -3426,8 +3793,12 @@
         <f t="shared" si="0"/>
         <v>0.23076923076923078</v>
       </c>
-    </row>
-    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J67" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D68">
         <v>100</v>
       </c>
@@ -3438,11 +3809,15 @@
         <v>75</v>
       </c>
       <c r="I68">
-        <f t="shared" ref="I68:I84" si="10">E68*(D68-F68)/((D68-E68)*F68)</f>
+        <f t="shared" ref="I68:I84" si="11">E68*(D68-F68)/((D68-E68)*F68)</f>
         <v>0.17948717948717949</v>
       </c>
-    </row>
-    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="J68" t="b">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D69">
         <v>100</v>
       </c>
@@ -3453,11 +3828,15 @@
         <v>80</v>
       </c>
       <c r="I69">
+        <f t="shared" si="11"/>
+        <v>0.13461538461538461</v>
+      </c>
+      <c r="J69" t="b">
         <f t="shared" si="10"/>
-        <v>0.13461538461538461</v>
-      </c>
-    </row>
-    <row r="70" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D70">
         <v>100</v>
       </c>
@@ -3468,11 +3847,15 @@
         <v>60</v>
       </c>
       <c r="I70">
+        <f t="shared" si="11"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="J70" t="b">
         <f t="shared" si="10"/>
-        <v>0.44444444444444442</v>
-      </c>
-    </row>
-    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D71">
         <v>100</v>
       </c>
@@ -3483,11 +3866,15 @@
         <v>65</v>
       </c>
       <c r="I71">
+        <f t="shared" si="11"/>
+        <v>0.35897435897435898</v>
+      </c>
+      <c r="J71" t="b">
         <f t="shared" si="10"/>
-        <v>0.35897435897435898</v>
-      </c>
-    </row>
-    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D72">
         <v>100</v>
       </c>
@@ -3498,11 +3885,15 @@
         <v>70</v>
       </c>
       <c r="I72">
+        <f t="shared" si="11"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="J72" t="b">
         <f t="shared" si="10"/>
-        <v>0.2857142857142857</v>
-      </c>
-    </row>
-    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D73">
         <v>100</v>
       </c>
@@ -3513,11 +3904,15 @@
         <v>75</v>
       </c>
       <c r="I73">
+        <f t="shared" si="11"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="J73" t="b">
         <f t="shared" si="10"/>
-        <v>0.22222222222222221</v>
-      </c>
-    </row>
-    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D74">
         <v>100</v>
       </c>
@@ -3528,11 +3923,15 @@
         <v>80</v>
       </c>
       <c r="I74">
+        <f t="shared" si="11"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J74" t="b">
         <f t="shared" si="10"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D75">
         <v>100</v>
       </c>
@@ -3543,11 +3942,15 @@
         <v>65</v>
       </c>
       <c r="I75">
+        <f t="shared" si="11"/>
+        <v>0.44055944055944057</v>
+      </c>
+      <c r="J75" t="b">
         <f t="shared" si="10"/>
-        <v>0.44055944055944057</v>
-      </c>
-    </row>
-    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D76">
         <v>100</v>
       </c>
@@ -3558,11 +3961,15 @@
         <v>70</v>
       </c>
       <c r="I76">
+        <f t="shared" si="11"/>
+        <v>0.35064935064935066</v>
+      </c>
+      <c r="J76" t="b">
         <f t="shared" si="10"/>
-        <v>0.35064935064935066</v>
-      </c>
-    </row>
-    <row r="77" spans="4:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D77">
         <v>100</v>
       </c>
@@ -3573,11 +3980,15 @@
         <v>75</v>
       </c>
       <c r="I77">
+        <f t="shared" si="11"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="J77" t="b">
         <f t="shared" si="10"/>
-        <v>0.27272727272727271</v>
-      </c>
-    </row>
-    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D78">
         <v>100</v>
       </c>
@@ -3588,11 +3999,15 @@
         <v>80</v>
       </c>
       <c r="I78">
+        <f t="shared" si="11"/>
+        <v>0.20454545454545456</v>
+      </c>
+      <c r="J78" t="b">
         <f t="shared" si="10"/>
-        <v>0.20454545454545456</v>
-      </c>
-    </row>
-    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D79">
         <v>100</v>
       </c>
@@ -3603,11 +4018,15 @@
         <v>70</v>
       </c>
       <c r="I79">
+        <f t="shared" si="11"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="J79" t="b">
         <f t="shared" si="10"/>
-        <v>0.42857142857142855</v>
-      </c>
-    </row>
-    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D80">
         <v>100</v>
       </c>
@@ -3618,11 +4037,15 @@
         <v>75</v>
       </c>
       <c r="I80">
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J80" t="b">
         <f t="shared" si="10"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D81">
         <v>100</v>
       </c>
@@ -3633,11 +4056,15 @@
         <v>80</v>
       </c>
       <c r="I81">
+        <f t="shared" si="11"/>
+        <v>0.25</v>
+      </c>
+      <c r="J81" t="b">
         <f t="shared" si="10"/>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D82">
         <v>100</v>
       </c>
@@ -3648,11 +4075,15 @@
         <v>75</v>
       </c>
       <c r="I82">
+        <f t="shared" si="11"/>
+        <v>0.40740740740740738</v>
+      </c>
+      <c r="J82" t="b">
         <f t="shared" si="10"/>
-        <v>0.40740740740740738</v>
-      </c>
-    </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D83">
         <v>100</v>
       </c>
@@ -3663,11 +4094,15 @@
         <v>80</v>
       </c>
       <c r="I83">
+        <f t="shared" si="11"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="J83" t="b">
         <f t="shared" si="10"/>
-        <v>0.30555555555555558</v>
-      </c>
-    </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D84">
         <v>100</v>
       </c>
@@ -3678,19 +4113,26 @@
         <v>80</v>
       </c>
       <c r="I84">
+        <f t="shared" si="11"/>
+        <v>0.375</v>
+      </c>
+      <c r="J84" t="b">
         <f t="shared" si="10"/>
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N88" t="s">
         <v>15</v>
       </c>
       <c r="O88" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P88" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>12</v>
       </c>
@@ -3713,27 +4155,31 @@
         <v>45</v>
       </c>
       <c r="I89">
-        <f t="shared" ref="I89" si="11">E89*(D89-F89)/((D89-E89)*F89)</f>
+        <f t="shared" ref="I89" si="12">E89*(D89-F89)/((D89-E89)*F89)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="J89">
-        <f t="shared" ref="J89" si="12">G89*(D89-H89)/((D89-G89)*H89)</f>
+        <f t="shared" ref="J89" si="13">G89*(D89-H89)/((D89-G89)*H89)</f>
         <v>0.40740740740740738</v>
       </c>
       <c r="K89">
-        <f t="shared" ref="K89" si="13">I89/J89</f>
+        <f t="shared" ref="K89" si="14">I89/J89</f>
         <v>1.0909090909090908</v>
       </c>
       <c r="L89">
-        <f t="shared" ref="L89" si="14">ABS(K89-1)</f>
+        <f t="shared" ref="L89" si="15">ABS(K89-1)</f>
         <v>9.0909090909090828E-2</v>
       </c>
       <c r="M89" t="b">
-        <f t="shared" ref="M89" si="15">NOT(OR(K89&lt;1,L89&lt;0.05))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M89" si="16">NOT(OR(K89&lt;1,L89&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P89" t="b">
+        <f>OR(E89=20,F89=80,G89=20,H89=80,F89-E89=20,H89-G89=20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C90">
         <v>35</v>
       </c>
@@ -3753,27 +4199,31 @@
         <v>55</v>
       </c>
       <c r="I90">
-        <f t="shared" ref="I90" si="16">E90*(D90-F90)/((D90-E90)*F90)</f>
+        <f t="shared" ref="I90" si="17">E90*(D90-F90)/((D90-E90)*F90)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="J90">
-        <f t="shared" ref="J90" si="17">G90*(D90-H90)/((D90-G90)*H90)</f>
+        <f t="shared" ref="J90" si="18">G90*(D90-H90)/((D90-G90)*H90)</f>
         <v>0.35064935064935066</v>
       </c>
       <c r="K90">
-        <f t="shared" ref="K90" si="18">I90/J90</f>
+        <f t="shared" ref="K90" si="19">I90/J90</f>
         <v>1.2674897119341564</v>
       </c>
       <c r="L90">
-        <f t="shared" ref="L90" si="19">ABS(K90-1)</f>
+        <f t="shared" ref="L90" si="20">ABS(K90-1)</f>
         <v>0.26748971193415638</v>
       </c>
       <c r="M90" t="b">
-        <f t="shared" ref="M90" si="20">NOT(OR(K90&lt;1,L90&lt;0.05))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M90" si="21">NOT(OR(K90&lt;1,L90&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P90" t="b">
+        <f t="shared" ref="P90:P139" si="22">OR(E90=20,F90=80,G90=20,H90=80,F90-E90=20,H90-G90=20)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>36</v>
       </c>
@@ -3793,30 +4243,34 @@
         <v>60</v>
       </c>
       <c r="I91">
-        <f t="shared" ref="I91" si="21">E91*(D91-F91)/((D91-E91)*F91)</f>
+        <f t="shared" ref="I91" si="23">E91*(D91-F91)/((D91-E91)*F91)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="J91">
-        <f t="shared" ref="J91" si="22">G91*(D91-H91)/((D91-G91)*H91)</f>
+        <f t="shared" ref="J91" si="24">G91*(D91-H91)/((D91-G91)*H91)</f>
         <v>0.35897435897435898</v>
       </c>
       <c r="K91">
-        <f t="shared" ref="K91" si="23">I91/J91</f>
+        <f t="shared" ref="K91" si="25">I91/J91</f>
         <v>1.2380952380952379</v>
       </c>
       <c r="L91">
-        <f t="shared" ref="L91" si="24">ABS(K91-1)</f>
+        <f t="shared" ref="L91" si="26">ABS(K91-1)</f>
         <v>0.23809523809523792</v>
       </c>
       <c r="M91" t="b">
-        <f t="shared" ref="M91" si="25">NOT(OR(K91&lt;1,L91&lt;0.05))</f>
+        <f t="shared" ref="M91" si="27">NOT(OR(K91&lt;1,L91&lt;0.05))</f>
         <v>1</v>
       </c>
       <c r="N91" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P91" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C92">
         <v>37</v>
       </c>
@@ -3836,27 +4290,31 @@
         <v>45</v>
       </c>
       <c r="I92">
-        <f t="shared" ref="I92:I98" si="26">E92*(D92-F92)/((D92-E92)*F92)</f>
+        <f t="shared" ref="I92:I98" si="28">E92*(D92-F92)/((D92-E92)*F92)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="J92">
-        <f t="shared" ref="J92:J98" si="27">G92*(D92-H92)/((D92-G92)*H92)</f>
+        <f t="shared" ref="J92:J98" si="29">G92*(D92-H92)/((D92-G92)*H92)</f>
         <v>0.30555555555555558</v>
       </c>
       <c r="K92">
-        <f t="shared" ref="K92:K98" si="28">I92/J92</f>
+        <f t="shared" ref="K92:K98" si="30">I92/J92</f>
         <v>1.4545454545454544</v>
       </c>
       <c r="L92">
-        <f t="shared" ref="L92:L98" si="29">ABS(K92-1)</f>
+        <f t="shared" ref="L92:L98" si="31">ABS(K92-1)</f>
         <v>0.45454545454545436</v>
       </c>
       <c r="M92" t="b">
-        <f t="shared" ref="M92:M98" si="30">NOT(OR(K92&lt;1,L92&lt;0.05))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M92:M98" si="32">NOT(OR(K92&lt;1,L92&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P92" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C93">
         <v>38</v>
       </c>
@@ -3876,30 +4334,34 @@
         <v>50</v>
       </c>
       <c r="I93">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J93">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.25</v>
       </c>
       <c r="K93">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>1.7777777777777777</v>
       </c>
       <c r="L93">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.77777777777777768</v>
       </c>
       <c r="M93" t="b">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="N93" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P93" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C94">
         <v>39</v>
       </c>
@@ -3919,27 +4381,31 @@
         <v>55</v>
       </c>
       <c r="I94">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J94">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="K94">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>2.1728395061728394</v>
       </c>
       <c r="L94">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>1.1728395061728394</v>
       </c>
       <c r="M94" t="b">
-        <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="P94" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C95">
         <v>40</v>
       </c>
@@ -3959,27 +4425,31 @@
         <v>70</v>
       </c>
       <c r="I95">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J95">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K95">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>3.1111111111111112</v>
       </c>
       <c r="L95">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>2.1111111111111112</v>
       </c>
       <c r="M95" t="b">
-        <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="P95" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C96">
         <v>41</v>
       </c>
@@ -3999,27 +4469,31 @@
         <v>75</v>
       </c>
       <c r="I96">
-        <f t="shared" ref="I96" si="31">E96*(D96-F96)/((D96-E96)*F96)</f>
+        <f t="shared" ref="I96" si="33">E96*(D96-F96)/((D96-E96)*F96)</f>
         <v>0.44444444444444442</v>
       </c>
       <c r="J96">
-        <f t="shared" ref="J96" si="32">G96*(D96-H96)/((D96-G96)*H96)</f>
+        <f t="shared" ref="J96" si="34">G96*(D96-H96)/((D96-G96)*H96)</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="K96">
-        <f t="shared" ref="K96" si="33">I96/J96</f>
+        <f t="shared" ref="K96" si="35">I96/J96</f>
         <v>4</v>
       </c>
       <c r="L96">
-        <f t="shared" ref="L96" si="34">ABS(K96-1)</f>
+        <f t="shared" ref="L96" si="36">ABS(K96-1)</f>
         <v>3</v>
       </c>
       <c r="M96" t="b">
-        <f t="shared" ref="M96" si="35">NOT(OR(K96&lt;1,L96&lt;0.05))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M96" si="37">NOT(OR(K96&lt;1,L96&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P96" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>42</v>
       </c>
@@ -4039,27 +4513,31 @@
         <v>80</v>
       </c>
       <c r="I97">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J97">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.10714285714285714</v>
       </c>
       <c r="K97">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>4.1481481481481479</v>
       </c>
       <c r="L97">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>3.1481481481481479</v>
       </c>
       <c r="M97" t="b">
-        <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="P97" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>43</v>
       </c>
@@ -4079,23 +4557,23 @@
         <v>80</v>
       </c>
       <c r="I98">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="J98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.25E-2</v>
       </c>
       <c r="K98">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>7.1111111111111107</v>
       </c>
       <c r="L98">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>6.1111111111111107</v>
       </c>
       <c r="M98" t="b">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="N98" t="s">
@@ -4104,8 +4582,12 @@
       <c r="O98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P98" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>44</v>
       </c>
@@ -4144,8 +4626,12 @@
         <f>NOT(OR(K99&lt;1,L99&lt;0.05))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P99" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>45</v>
       </c>
@@ -4184,8 +4670,12 @@
         <f>NOT(OR(K100&lt;1,L100&lt;0.05))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P100" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C101">
         <v>46</v>
       </c>
@@ -4205,27 +4695,31 @@
         <v>45</v>
       </c>
       <c r="I101">
-        <f t="shared" ref="I101:I108" si="36">E101*(D101-F101)/((D101-E101)*F101)</f>
+        <f t="shared" ref="I101:I108" si="38">E101*(D101-F101)/((D101-E101)*F101)</f>
         <v>0.40740740740740738</v>
       </c>
       <c r="J101">
-        <f t="shared" ref="J101:J108" si="37">G101*(D101-H101)/((D101-G101)*H101)</f>
+        <f t="shared" ref="J101:J108" si="39">G101*(D101-H101)/((D101-G101)*H101)</f>
         <v>0.30555555555555558</v>
       </c>
       <c r="K101">
-        <f t="shared" ref="K101:K108" si="38">I101/J101</f>
+        <f t="shared" ref="K101:K108" si="40">I101/J101</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="L101">
-        <f t="shared" ref="L101:L108" si="39">ABS(K101-1)</f>
+        <f t="shared" ref="L101:L108" si="41">ABS(K101-1)</f>
         <v>0.33333333333333326</v>
       </c>
       <c r="M101" t="b">
-        <f t="shared" ref="M101:M108" si="40">NOT(OR(K101&lt;1,L101&lt;0.05))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M101:M108" si="42">NOT(OR(K101&lt;1,L101&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P101" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C102">
         <v>47</v>
       </c>
@@ -4245,27 +4739,31 @@
         <v>50</v>
       </c>
       <c r="I102">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="J102">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.25</v>
       </c>
       <c r="K102">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>1.6296296296296295</v>
       </c>
       <c r="L102">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.62962962962962954</v>
       </c>
       <c r="M102" t="b">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="P102" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C103">
         <v>48</v>
       </c>
@@ -4285,30 +4783,34 @@
         <v>55</v>
       </c>
       <c r="I103">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="J103">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="K103">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>1.9917695473251027</v>
       </c>
       <c r="L103">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.9917695473251027</v>
       </c>
       <c r="M103" t="b">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="N103" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="104" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P103" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C104">
         <v>49</v>
       </c>
@@ -4328,27 +4830,31 @@
         <v>70</v>
       </c>
       <c r="I104">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="J104">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K104">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>2.8518518518518516</v>
       </c>
       <c r="L104">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>1.8518518518518516</v>
       </c>
       <c r="M104" t="b">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="P104" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>50</v>
       </c>
@@ -4368,27 +4874,31 @@
         <v>75</v>
       </c>
       <c r="I105">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="J105">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="K105">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="L105">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="M105" t="b">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="P105" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>51</v>
       </c>
@@ -4408,27 +4918,31 @@
         <v>80</v>
       </c>
       <c r="I106">
-        <f t="shared" ref="I106" si="41">E106*(D106-F106)/((D106-E106)*F106)</f>
+        <f t="shared" ref="I106" si="43">E106*(D106-F106)/((D106-E106)*F106)</f>
         <v>0.40740740740740738</v>
       </c>
       <c r="J106">
-        <f t="shared" ref="J106" si="42">G106*(D106-H106)/((D106-G106)*H106)</f>
+        <f t="shared" ref="J106" si="44">G106*(D106-H106)/((D106-G106)*H106)</f>
         <v>0.10714285714285714</v>
       </c>
       <c r="K106">
-        <f t="shared" ref="K106" si="43">I106/J106</f>
+        <f t="shared" ref="K106" si="45">I106/J106</f>
         <v>3.8024691358024691</v>
       </c>
       <c r="L106">
-        <f t="shared" ref="L106" si="44">ABS(K106-1)</f>
+        <f t="shared" ref="L106" si="46">ABS(K106-1)</f>
         <v>2.8024691358024691</v>
       </c>
       <c r="M106" t="b">
-        <f t="shared" ref="M106" si="45">NOT(OR(K106&lt;1,L106&lt;0.05))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M106" si="47">NOT(OR(K106&lt;1,L106&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P106" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>52</v>
       </c>
@@ -4448,27 +4962,31 @@
         <v>80</v>
       </c>
       <c r="I107">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.40740740740740738</v>
       </c>
       <c r="J107">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>6.25E-2</v>
       </c>
       <c r="K107">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>6.5185185185185182</v>
       </c>
       <c r="L107">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>5.5185185185185182</v>
       </c>
       <c r="M107" t="b">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="P107" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>53</v>
       </c>
@@ -4488,27 +5006,31 @@
         <v>45</v>
       </c>
       <c r="I108">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.35064935064935066</v>
       </c>
       <c r="J108">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.30555555555555558</v>
       </c>
       <c r="K108">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>1.1475796930342383</v>
       </c>
       <c r="L108">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.14757969303423835</v>
       </c>
       <c r="M108" t="b">
-        <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="P108" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>54</v>
       </c>
@@ -4528,27 +5050,31 @@
         <v>50</v>
       </c>
       <c r="I109">
-        <f t="shared" ref="I109:I129" si="46">E109*(D109-F109)/((D109-E109)*F109)</f>
+        <f t="shared" ref="I109:I128" si="48">E109*(D109-F109)/((D109-E109)*F109)</f>
         <v>0.35064935064935066</v>
       </c>
       <c r="J109">
-        <f t="shared" ref="J109:J129" si="47">G109*(D109-H109)/((D109-G109)*H109)</f>
+        <f t="shared" ref="J109:J128" si="49">G109*(D109-H109)/((D109-G109)*H109)</f>
         <v>0.25</v>
       </c>
       <c r="K109">
-        <f t="shared" ref="K109:K129" si="48">I109/J109</f>
+        <f t="shared" ref="K109:K135" si="50">I109/J109</f>
         <v>1.4025974025974026</v>
       </c>
       <c r="L109">
-        <f t="shared" ref="L109:L129" si="49">ABS(K109-1)</f>
+        <f t="shared" ref="L109:L135" si="51">ABS(K109-1)</f>
         <v>0.40259740259740262</v>
       </c>
       <c r="M109" t="b">
-        <f t="shared" ref="M109:M129" si="50">NOT(OR(K109&lt;1,L109&lt;0.05))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M109:M135" si="52">NOT(OR(K109&lt;1,L109&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P109" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C110">
         <v>55</v>
       </c>
@@ -4568,30 +5094,34 @@
         <v>55</v>
       </c>
       <c r="I110">
-        <f t="shared" ref="I110" si="51">E110*(D110-F110)/((D110-E110)*F110)</f>
+        <f t="shared" ref="I110" si="53">E110*(D110-F110)/((D110-E110)*F110)</f>
         <v>0.35064935064935066</v>
       </c>
       <c r="J110">
-        <f t="shared" ref="J110" si="52">G110*(D110-H110)/((D110-G110)*H110)</f>
+        <f t="shared" ref="J110" si="54">G110*(D110-H110)/((D110-G110)*H110)</f>
         <v>0.27272727272727271</v>
       </c>
       <c r="K110">
-        <f t="shared" ref="K110" si="53">I110/J110</f>
+        <f t="shared" ref="K110" si="55">I110/J110</f>
         <v>1.2857142857142858</v>
       </c>
       <c r="L110">
-        <f t="shared" ref="L110" si="54">ABS(K110-1)</f>
+        <f t="shared" ref="L110" si="56">ABS(K110-1)</f>
         <v>0.28571428571428581</v>
       </c>
       <c r="M110" t="b">
-        <f t="shared" ref="M110" si="55">NOT(OR(K110&lt;1,L110&lt;0.05))</f>
+        <f t="shared" ref="M110" si="57">NOT(OR(K110&lt;1,L110&lt;0.05))</f>
         <v>1</v>
       </c>
       <c r="N110" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="111" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P110" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C111">
         <v>56</v>
       </c>
@@ -4611,27 +5141,31 @@
         <v>55</v>
       </c>
       <c r="I111">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.35064935064935066</v>
       </c>
       <c r="J111">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="K111">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.7142857142857142</v>
       </c>
       <c r="L111">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.71428571428571419</v>
       </c>
       <c r="M111" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P111" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C112">
         <v>57</v>
       </c>
@@ -4651,23 +5185,23 @@
         <v>70</v>
       </c>
       <c r="I112">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.35064935064935066</v>
       </c>
       <c r="J112">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K112">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>2.4545454545454546</v>
       </c>
       <c r="L112">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>1.4545454545454546</v>
       </c>
       <c r="M112" t="b">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="N112" t="s">
@@ -4676,8 +5210,12 @@
       <c r="O112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P112" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C113">
         <v>58</v>
       </c>
@@ -4697,27 +5235,31 @@
         <v>75</v>
       </c>
       <c r="I113">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.35064935064935066</v>
       </c>
       <c r="J113">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="K113">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>3.1558441558441559</v>
       </c>
       <c r="L113">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>2.1558441558441559</v>
       </c>
       <c r="M113" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P113" t="b">
+        <f>OR(E113=20,F113=80,G113=20,H113=80,F113-E113=20,H113-G113=20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C114">
         <v>59</v>
       </c>
@@ -4737,27 +5279,31 @@
         <v>80</v>
       </c>
       <c r="I114">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.35064935064935066</v>
       </c>
       <c r="J114">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6.25E-2</v>
       </c>
       <c r="K114">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>5.6103896103896105</v>
       </c>
       <c r="L114">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>4.6103896103896105</v>
       </c>
       <c r="M114" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P114" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C115">
         <v>60</v>
       </c>
@@ -4777,30 +5323,34 @@
         <v>50</v>
       </c>
       <c r="I115">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.30555555555555558</v>
       </c>
       <c r="J115">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.25</v>
       </c>
       <c r="K115">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.2222222222222223</v>
       </c>
       <c r="L115">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.22222222222222232</v>
       </c>
       <c r="M115" t="b">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="O115">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P115" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C116">
         <v>61</v>
       </c>
@@ -4820,23 +5370,23 @@
         <v>55</v>
       </c>
       <c r="I116">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.30555555555555558</v>
       </c>
       <c r="J116">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="K116">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.4938271604938271</v>
       </c>
       <c r="L116">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.49382716049382713</v>
       </c>
       <c r="M116" t="b">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="N116" t="s">
@@ -4845,8 +5395,12 @@
       <c r="O116">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P116" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C117">
         <v>62</v>
       </c>
@@ -4866,27 +5420,31 @@
         <v>70</v>
       </c>
       <c r="I117">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.30555555555555558</v>
       </c>
       <c r="J117">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K117">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>2.1388888888888893</v>
       </c>
       <c r="L117">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>1.1388888888888893</v>
       </c>
       <c r="M117" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P117" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C118">
         <v>63</v>
       </c>
@@ -4906,27 +5464,31 @@
         <v>75</v>
       </c>
       <c r="I118">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.30555555555555558</v>
       </c>
       <c r="J118">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="K118">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>2.7500000000000004</v>
       </c>
       <c r="L118">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>1.7500000000000004</v>
       </c>
       <c r="M118" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P118" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C119">
         <v>64</v>
       </c>
@@ -4946,30 +5508,34 @@
         <v>80</v>
       </c>
       <c r="I119">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.30555555555555558</v>
       </c>
       <c r="J119">
-        <f t="shared" si="47"/>
+        <f>G119*(D119-H119)/((D119-G119)*H119)</f>
         <v>6.25E-2</v>
       </c>
       <c r="K119">
-        <f t="shared" si="48"/>
+        <f>I119/J119</f>
         <v>4.8888888888888893</v>
       </c>
       <c r="L119">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>3.8888888888888893</v>
       </c>
       <c r="M119" t="b">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="N119" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="120" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P119" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C120">
         <v>65</v>
       </c>
@@ -4989,30 +5555,34 @@
         <v>55</v>
       </c>
       <c r="I120">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.25</v>
       </c>
       <c r="J120">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="K120">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.2222222222222221</v>
       </c>
       <c r="L120">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.2222222222222221</v>
       </c>
       <c r="M120" t="b">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="O120">
         <v>3</v>
       </c>
-    </row>
-    <row r="121" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="P120" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>66</v>
       </c>
@@ -5032,27 +5602,31 @@
         <v>70</v>
       </c>
       <c r="I121">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.25</v>
       </c>
       <c r="J121">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K121">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.75</v>
       </c>
       <c r="L121">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.75</v>
       </c>
       <c r="M121" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P121" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C122">
         <v>67</v>
       </c>
@@ -5072,30 +5646,34 @@
         <v>75</v>
       </c>
       <c r="I122">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.25</v>
       </c>
       <c r="J122">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="K122">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>2.25</v>
       </c>
       <c r="L122">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>1.25</v>
       </c>
       <c r="M122" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-      <c r="N122" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="123" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="O122" t="s">
+        <v>19</v>
+      </c>
+      <c r="P122" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C123">
         <v>68</v>
       </c>
@@ -5115,27 +5693,31 @@
         <v>80</v>
       </c>
       <c r="I123">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.25</v>
       </c>
       <c r="J123">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6.25E-2</v>
       </c>
       <c r="K123">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>4</v>
       </c>
       <c r="L123">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>3</v>
       </c>
       <c r="M123" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P123" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C124">
         <v>69</v>
       </c>
@@ -5155,30 +5737,34 @@
         <v>70</v>
       </c>
       <c r="I124">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="J124">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="K124">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.4318181818181819</v>
       </c>
       <c r="L124">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.43181818181818188</v>
       </c>
       <c r="M124" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-      <c r="N124" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="125" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="O124" t="s">
+        <v>20</v>
+      </c>
+      <c r="P124" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C125">
         <v>70</v>
       </c>
@@ -5198,27 +5784,31 @@
         <v>75</v>
       </c>
       <c r="I125">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="J125">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="K125">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.8409090909090911</v>
       </c>
       <c r="L125">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.84090909090909105</v>
       </c>
       <c r="M125" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P125" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C126">
         <v>71</v>
       </c>
@@ -5238,27 +5828,31 @@
         <v>80</v>
       </c>
       <c r="I126">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.20454545454545456</v>
       </c>
       <c r="J126">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6.25E-2</v>
       </c>
       <c r="K126">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>3.2727272727272729</v>
       </c>
       <c r="L126">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>2.2727272727272729</v>
       </c>
       <c r="M126" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P126" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C127">
         <v>72</v>
       </c>
@@ -5278,27 +5872,34 @@
         <v>75</v>
       </c>
       <c r="I127">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="J127">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="K127">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.2857142857142858</v>
       </c>
       <c r="L127">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.28571428571428581</v>
       </c>
       <c r="M127" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="3:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="N127" t="s">
+        <v>13</v>
+      </c>
+      <c r="P127" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C128">
         <v>73</v>
       </c>
@@ -5318,30 +5919,31 @@
         <v>80</v>
       </c>
       <c r="I128">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="J128">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6.25E-2</v>
       </c>
       <c r="K128">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>2.2857142857142856</v>
       </c>
       <c r="L128">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>1.2857142857142856</v>
       </c>
       <c r="M128" t="b">
-        <f t="shared" si="50"/>
-        <v>1</v>
-      </c>
-      <c r="N128" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="129" spans="3:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P128" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C129">
         <v>74</v>
       </c>
@@ -5361,45 +5963,501 @@
         <v>80</v>
       </c>
       <c r="I129">
-        <f t="shared" si="46"/>
+        <f>E129*(D129-F129)/((D129-E129)*F129)</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="J129">
-        <f t="shared" si="47"/>
+        <f>G129*(D129-H129)/((D129-G129)*H129)</f>
         <v>6.25E-2</v>
       </c>
       <c r="K129">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.7777777777777777</v>
       </c>
       <c r="L129">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.77777777777777768</v>
       </c>
       <c r="M129" t="b">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P129" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C130">
+        <v>75</v>
+      </c>
+      <c r="D130">
+        <v>100</v>
+      </c>
+      <c r="E130">
+        <v>35</v>
+      </c>
+      <c r="F130">
+        <v>65</v>
+      </c>
+      <c r="G130">
+        <v>30</v>
+      </c>
+      <c r="H130">
+        <v>65</v>
+      </c>
+      <c r="I130">
+        <f t="shared" ref="I130:I135" si="58">E130*(D130-F130)/((D130-E130)*F130)</f>
+        <v>0.28994082840236685</v>
+      </c>
+      <c r="J130">
+        <f t="shared" ref="J130:J135" si="59">G130*(D130-H130)/((D130-G130)*H130)</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="K130">
         <f t="shared" si="50"/>
-        <v>1</v>
+        <v>1.2564102564102562</v>
+      </c>
+      <c r="L130">
+        <f t="shared" si="51"/>
+        <v>0.25641025641025617</v>
+      </c>
+      <c r="M130" t="b">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P130" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C131">
+        <v>76</v>
+      </c>
+      <c r="D131">
+        <v>100</v>
+      </c>
+      <c r="E131">
+        <v>35</v>
+      </c>
+      <c r="F131">
+        <v>65</v>
+      </c>
+      <c r="G131">
+        <v>25</v>
+      </c>
+      <c r="H131">
+        <v>60</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="58"/>
+        <v>0.28994082840236685</v>
+      </c>
+      <c r="J131">
+        <f t="shared" si="59"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="K131">
+        <f t="shared" si="50"/>
+        <v>1.3047337278106508</v>
+      </c>
+      <c r="L131">
+        <f t="shared" si="51"/>
+        <v>0.30473372781065078</v>
+      </c>
+      <c r="M131" t="b">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P131" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <v>77</v>
+      </c>
+      <c r="D132">
+        <v>100</v>
+      </c>
+      <c r="E132">
+        <v>35</v>
+      </c>
+      <c r="F132">
+        <v>65</v>
+      </c>
+      <c r="G132">
+        <v>30</v>
+      </c>
+      <c r="H132">
+        <v>70</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="58"/>
+        <v>0.28994082840236685</v>
+      </c>
+      <c r="J132">
+        <f t="shared" si="59"/>
+        <v>0.18367346938775511</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="50"/>
+        <v>1.578566732412886</v>
+      </c>
+      <c r="L132">
+        <f t="shared" si="51"/>
+        <v>0.57856673241288603</v>
+      </c>
+      <c r="M132" t="b">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P132" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C133">
+        <v>78</v>
+      </c>
+      <c r="D133">
+        <v>100</v>
+      </c>
+      <c r="E133">
+        <v>35</v>
+      </c>
+      <c r="F133">
+        <v>65</v>
+      </c>
+      <c r="G133">
+        <v>25</v>
+      </c>
+      <c r="H133">
+        <v>70</v>
+      </c>
+      <c r="I133">
+        <f t="shared" si="58"/>
+        <v>0.28994082840236685</v>
+      </c>
+      <c r="J133">
+        <f t="shared" si="59"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K133">
+        <f t="shared" si="50"/>
+        <v>2.029585798816568</v>
+      </c>
+      <c r="L133">
+        <f t="shared" si="51"/>
+        <v>1.029585798816568</v>
+      </c>
+      <c r="M133" t="b">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P133" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <v>79</v>
+      </c>
+      <c r="D134">
+        <v>100</v>
+      </c>
+      <c r="E134">
+        <v>35</v>
+      </c>
+      <c r="F134">
+        <v>65</v>
+      </c>
+      <c r="G134">
+        <v>25</v>
+      </c>
+      <c r="H134">
+        <v>75</v>
+      </c>
+      <c r="I134">
+        <f t="shared" si="58"/>
+        <v>0.28994082840236685</v>
+      </c>
+      <c r="J134">
+        <f t="shared" si="59"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K134">
+        <f t="shared" si="50"/>
+        <v>2.6094674556213016</v>
+      </c>
+      <c r="L134">
+        <f t="shared" si="51"/>
+        <v>1.6094674556213016</v>
+      </c>
+      <c r="M134" t="b">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="N134" t="s">
+        <v>13</v>
+      </c>
+      <c r="O134" t="s">
+        <v>18</v>
+      </c>
+      <c r="P134" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <v>80</v>
+      </c>
+      <c r="D135">
+        <v>100</v>
+      </c>
+      <c r="E135">
+        <v>30</v>
+      </c>
+      <c r="F135">
+        <v>65</v>
+      </c>
+      <c r="G135">
+        <v>30</v>
+      </c>
+      <c r="H135">
+        <v>70</v>
+      </c>
+      <c r="I135">
+        <f t="shared" si="58"/>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="J135">
+        <f t="shared" si="59"/>
+        <v>0.18367346938775511</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="50"/>
+        <v>1.2564102564102564</v>
+      </c>
+      <c r="L135">
+        <f t="shared" si="51"/>
+        <v>0.25641025641025639</v>
+      </c>
+      <c r="M135" t="b">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P135" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <v>81</v>
+      </c>
+      <c r="D136">
+        <v>100</v>
+      </c>
+      <c r="E136">
+        <v>30</v>
+      </c>
+      <c r="F136">
+        <v>65</v>
+      </c>
+      <c r="G136">
+        <v>25</v>
+      </c>
+      <c r="H136">
+        <v>70</v>
+      </c>
+      <c r="I136">
+        <f t="shared" ref="I136:I140" si="60">E136*(D136-F136)/((D136-E136)*F136)</f>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="J136">
+        <f t="shared" ref="J136:J140" si="61">G136*(D136-H136)/((D136-G136)*H136)</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K136">
+        <f t="shared" ref="K136:K140" si="62">I136/J136</f>
+        <v>1.6153846153846156</v>
+      </c>
+      <c r="L136">
+        <f t="shared" ref="L136:L140" si="63">ABS(K136-1)</f>
+        <v>0.61538461538461564</v>
+      </c>
+      <c r="M136" t="b">
+        <f t="shared" ref="M136:M140" si="64">NOT(OR(K136&lt;1,L136&lt;0.05))</f>
+        <v>1</v>
+      </c>
+      <c r="P136" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C137">
+        <v>82</v>
+      </c>
+      <c r="D137">
+        <v>100</v>
+      </c>
+      <c r="E137">
+        <v>30</v>
+      </c>
+      <c r="F137">
+        <v>65</v>
+      </c>
+      <c r="G137">
+        <v>25</v>
+      </c>
+      <c r="H137">
+        <v>75</v>
+      </c>
+      <c r="I137">
+        <f t="shared" si="60"/>
+        <v>0.23076923076923078</v>
+      </c>
+      <c r="J137">
+        <f t="shared" si="61"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="62"/>
+        <v>2.0769230769230771</v>
+      </c>
+      <c r="L137">
+        <f t="shared" si="63"/>
+        <v>1.0769230769230771</v>
+      </c>
+      <c r="M137" t="b">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="P137" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C138">
+        <v>83</v>
+      </c>
+      <c r="D138">
+        <v>100</v>
+      </c>
+      <c r="E138">
+        <v>30</v>
+      </c>
+      <c r="F138">
+        <v>70</v>
+      </c>
+      <c r="G138">
+        <v>25</v>
+      </c>
+      <c r="H138">
+        <v>70</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="60"/>
+        <v>0.18367346938775511</v>
+      </c>
+      <c r="J138">
+        <f t="shared" si="61"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="K138">
+        <f t="shared" si="62"/>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="L138">
+        <f t="shared" si="63"/>
+        <v>0.28571428571428581</v>
+      </c>
+      <c r="M138" t="b">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="N138" t="s">
+        <v>13</v>
+      </c>
+      <c r="O138" t="s">
+        <v>17</v>
+      </c>
+      <c r="P138" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C139">
+        <v>84</v>
+      </c>
+      <c r="D139">
+        <v>100</v>
+      </c>
+      <c r="E139">
+        <v>30</v>
+      </c>
+      <c r="F139">
+        <v>70</v>
+      </c>
+      <c r="G139">
+        <v>25</v>
+      </c>
+      <c r="H139">
+        <v>75</v>
+      </c>
+      <c r="I139">
+        <f t="shared" si="60"/>
+        <v>0.18367346938775511</v>
+      </c>
+      <c r="J139">
+        <f t="shared" si="61"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="K139">
+        <f t="shared" si="62"/>
+        <v>1.6530612244897962</v>
+      </c>
+      <c r="L139">
+        <f t="shared" si="63"/>
+        <v>0.6530612244897962</v>
+      </c>
+      <c r="M139" t="b">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="P139" t="b">
+        <f t="shared" si="22"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="W8:W37 L89:L129">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="lessThan">
+  <conditionalFormatting sqref="W8:W37 L89:L140">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V8:V37 K89:K129">
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="lessThan">
+  <conditionalFormatting sqref="V8:V37 K89:K140">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N37">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5411,25 +6469,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K37">
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:L37">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M37 M89:M129">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+  <conditionalFormatting sqref="M4:M37 M89:M140">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:I84">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5441,7 +6499,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J37">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5452,8 +6510,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I89:I129">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="I89:I140">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5464,8 +6522,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J89:J129">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="J89:J140">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5476,7 +6534,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J40:J84">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P89:P139">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>